<commit_message>
Added a column to the database; Added a combobox widget with information about the type of product.
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
@@ -23,12 +23,6 @@
   </si>
   <si>
     <t>Date_time</t>
-  </si>
-  <si>
-    <t>Milk</t>
-  </si>
-  <si>
-    <t>2022-11-05 13:03:10</t>
   </si>
 </sst>
 </file>
@@ -386,13 +380,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="2:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,20 +397,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes in the clicked_btn_get method: added data migration by product type
</commit_message>
<xml_diff>
--- a/Orders.xlsx
+++ b/Orders.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -24,12 +24,15 @@
   <si>
     <t>Date_time</t>
   </si>
+  <si>
+    <t>Type_prod</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,24 +84,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -136,7 +147,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,6 +181,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -204,9 +216,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -379,14 +392,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,6 +416,9 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>